<commit_message>
Reuse compressor_3_2 submodule in booth2_pp_compressor module
</commit_message>
<xml_diff>
--- a/doc/compress_example.xlsx
+++ b/doc/compress_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lau Chinyuan\Desktop\Huawei\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CE50B0-544E-4DC8-A563-0789E85E9BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E072F3-B4BF-4EE3-933A-F73CDF41A935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{1DE01F21-B836-4509-9EF7-59739B22F2E4}"/>
+    <workbookView xWindow="43080" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{1DE01F21-B836-4509-9EF7-59739B22F2E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="201">
   <si>
     <t>PP1</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -187,9 +187,6 @@
     <t>1Cin[6] = 0</t>
   </si>
   <si>
-    <t>1C[29]</t>
-  </si>
-  <si>
     <t>1C[28]</t>
   </si>
   <si>
@@ -260,277 +257,482 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>2C[28]</t>
+  </si>
+  <si>
+    <t>2C[27]</t>
+  </si>
+  <si>
+    <t>2C[26]</t>
+  </si>
+  <si>
+    <t>2C[25]</t>
+  </si>
+  <si>
+    <t>2C[24]</t>
+  </si>
+  <si>
+    <t>2C[23]</t>
+  </si>
+  <si>
+    <t>2C[22]</t>
+  </si>
+  <si>
+    <t>2C[21]</t>
+  </si>
+  <si>
+    <t>2C[20]</t>
+  </si>
+  <si>
+    <t>2C[19]</t>
+  </si>
+  <si>
+    <t>2C[18]</t>
+  </si>
+  <si>
+    <t>2C[17]</t>
+  </si>
+  <si>
+    <t>2C[16]</t>
+  </si>
+  <si>
+    <t>2C[15]</t>
+  </si>
+  <si>
+    <t>2C[14]</t>
+  </si>
+  <si>
+    <t>2C[13]</t>
+  </si>
+  <si>
+    <t>2C[12]</t>
+  </si>
+  <si>
+    <t>2C[11]</t>
+  </si>
+  <si>
+    <t>2C[10]</t>
+  </si>
+  <si>
+    <t>2C[9]</t>
+  </si>
+  <si>
+    <t>2C[8]</t>
+  </si>
+  <si>
+    <t>2D[9]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[30]</t>
+  </si>
+  <si>
+    <t>2D[29]</t>
+  </si>
+  <si>
+    <t>2D[28]</t>
+  </si>
+  <si>
+    <t>2D[27]</t>
+  </si>
+  <si>
+    <t>2D[25]</t>
+  </si>
+  <si>
+    <t>2D[24]</t>
+  </si>
+  <si>
+    <t>2D[23]</t>
+  </si>
+  <si>
+    <t>2D[22]</t>
+  </si>
+  <si>
+    <t>2D[21]</t>
+  </si>
+  <si>
+    <t>2D[20]</t>
+  </si>
+  <si>
+    <t>2D[19]</t>
+  </si>
+  <si>
+    <t>2D[18]</t>
+  </si>
+  <si>
+    <t>2D[17]</t>
+  </si>
+  <si>
+    <t>2D[16]</t>
+  </si>
+  <si>
+    <t>2D[15]</t>
+  </si>
+  <si>
+    <t>2D[14]</t>
+  </si>
+  <si>
+    <t>2D[13]</t>
+  </si>
+  <si>
+    <t>2D[12]</t>
+  </si>
+  <si>
+    <t>2D[11]</t>
+  </si>
+  <si>
+    <t>2D[10]</t>
+  </si>
+  <si>
+    <t>PPC1_1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPC1_2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPC1_3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPC1_4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPC2_1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPC2_2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2cin[10] = 0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>图例说明</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>图样</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>说明</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>符号扩展</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用4-2压缩</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用3-2压缩</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>补零</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1D[i]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一级压缩器的在第i位权重位置的和输出</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>注意这里的1C[i]或者1D[i]与上面几行里的数值不相同，这里只是表达位置关系，二者数据不同</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2Cin[i] = 2Co[i-1]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[26]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1D[13]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1Cin[i] = 1Co[i-1]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>这一部分的4：2压缩完全可以使用23位的一个4：2压缩替代,因为其输入输出关系是一样的</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用精简版4：2(只输出本位权重，实际上是异或)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>最高位符号位由输入的两个数据的高位异或得到</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>由4：2压缩后的数据扩展得到</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一级处理得到PPC1_1 PPC2_1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第二级处理得到PPC2_1 PPC2_2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第二级处理得到PPC2_1 PPC2_2过程</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>author:LauChinyuan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>lauchinyuan@yeah.net</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1C[4]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1C[5]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用两个异或门实现</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[29]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[28]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[27]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[25]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[24]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[23]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[22]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[21]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[20]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[19]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[18]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[17]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[16]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[15]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[14]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[13]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[12]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[11]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[10]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C[28]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C[27]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C[26]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C[25]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C[24]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C[23]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C[22]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C[21]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C[20]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C[19]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C[18]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C[17]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C[16]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C[15]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C[14]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C[13]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C[12]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C[11]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C[10]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C[9]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C[8]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用外部异或门&amp;与非门,高位可以复用</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1C[20]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一级处理得到PPC1_1 PPC1_2过程</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一级处理PPC1_3 PPC1_4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一次处理PPC1_3 PPC1_4过程</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用外部异或门&amp;与非门,高位部分积的产生可以复用这一结果</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用不考虑进位输入的4:2压缩器</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1C[21]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1D[31]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1D[30]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[30]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D[31]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>2C[29]</t>
-  </si>
-  <si>
-    <t>2C[28]</t>
-  </si>
-  <si>
-    <t>2C[27]</t>
-  </si>
-  <si>
-    <t>2C[26]</t>
-  </si>
-  <si>
-    <t>2C[25]</t>
-  </si>
-  <si>
-    <t>2C[24]</t>
-  </si>
-  <si>
-    <t>2C[23]</t>
-  </si>
-  <si>
-    <t>2C[22]</t>
-  </si>
-  <si>
-    <t>2C[21]</t>
-  </si>
-  <si>
-    <t>2C[20]</t>
-  </si>
-  <si>
-    <t>2C[19]</t>
-  </si>
-  <si>
-    <t>2C[18]</t>
-  </si>
-  <si>
-    <t>2C[17]</t>
-  </si>
-  <si>
-    <t>2C[16]</t>
-  </si>
-  <si>
-    <t>2C[15]</t>
-  </si>
-  <si>
-    <t>2C[14]</t>
-  </si>
-  <si>
-    <t>2C[13]</t>
-  </si>
-  <si>
-    <t>2C[12]</t>
-  </si>
-  <si>
-    <t>2C[11]</t>
-  </si>
-  <si>
-    <t>2C[10]</t>
-  </si>
-  <si>
-    <t>2C[9]</t>
-  </si>
-  <si>
-    <t>2C[8]</t>
-  </si>
-  <si>
-    <t>2D[9]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2D[30]</t>
-  </si>
-  <si>
-    <t>2D[29]</t>
-  </si>
-  <si>
-    <t>2D[28]</t>
-  </si>
-  <si>
-    <t>2D[27]</t>
-  </si>
-  <si>
-    <t>2D[25]</t>
-  </si>
-  <si>
-    <t>2D[24]</t>
-  </si>
-  <si>
-    <t>2D[23]</t>
-  </si>
-  <si>
-    <t>2D[22]</t>
-  </si>
-  <si>
-    <t>2D[21]</t>
-  </si>
-  <si>
-    <t>2D[20]</t>
-  </si>
-  <si>
-    <t>2D[19]</t>
-  </si>
-  <si>
-    <t>2D[18]</t>
-  </si>
-  <si>
-    <t>2D[17]</t>
-  </si>
-  <si>
-    <t>2D[16]</t>
-  </si>
-  <si>
-    <t>2D[15]</t>
-  </si>
-  <si>
-    <t>2D[14]</t>
-  </si>
-  <si>
-    <t>2D[13]</t>
-  </si>
-  <si>
-    <t>2D[12]</t>
-  </si>
-  <si>
-    <t>2D[11]</t>
-  </si>
-  <si>
-    <t>2D[10]</t>
-  </si>
-  <si>
-    <t>PPC1_1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PPC1_2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PPC1_3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PPC1_4</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PPC2_1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PPC2_2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2cin[10] = 0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>结果</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>图例说明</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>图样</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>说明</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>符号扩展</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用4-2压缩</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用3-2压缩</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>补零</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1D[i]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>第一级压缩器的在第i位权重位置的和输出</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>注意这里的1C[i]或者1D[i]与上面几行里的数值不相同，这里只是表达位置关系，二者数据不同</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2Cin[i] = 2Co[i-1]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2D[26]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1D[13]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1Cin[i] = 1Co[i-1]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>这一部分的4：2压缩完全可以使用23位的一个4：2压缩替代,因为其输入输出关系是一样的</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用精简版4：2(只输出本位权重，实际上是异或)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1C[23]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>最高位符号位由输入的两个数据的高位异或得到</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>由4：2压缩后的数据扩展得到</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>第一级处理PPC1_3 PPC2_4</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>第一次处理PPC1_3 PPC2_4过程</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>第一级处理得到PPC1_1 PPC2_1过程</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>第一级处理得到PPC1_1 PPC2_1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>第二级处理得到PPC2_1 PPC2_2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>第二级处理得到PPC2_1 PPC2_2过程</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>符号位由乘数和被乘数异或得到</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>author:LauChinyuan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>lauchinyuan@yeah.net</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2C[30]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1C[28]</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -589,7 +791,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -650,8 +852,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -711,6 +937,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -720,7 +1026,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -793,6 +1099,30 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -803,6 +1133,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1120,10 +1477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DCD4167-9BB9-470D-B17A-532D76D71D0D}">
-  <dimension ref="A1:AH83"/>
+  <dimension ref="A1:AH87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="W72" sqref="W72"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1135,26 +1492,32 @@
     <col min="5" max="5" width="7.265625" style="15" customWidth="1"/>
     <col min="6" max="6" width="7.265625" style="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="9.06640625" style="15"/>
-    <col min="14" max="14" width="12.1328125" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="9.06640625" style="15"/>
+    <col min="8" max="8" width="9.06640625" style="15"/>
+    <col min="9" max="9" width="6.9296875" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="9.06640625" style="15"/>
+    <col min="14" max="14" width="6.73046875" style="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="57.06640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="9.06640625" style="15"/>
     <col min="19" max="19" width="23.59765625" style="15" customWidth="1"/>
     <col min="20" max="20" width="9.06640625" style="15"/>
     <col min="21" max="21" width="6.73046875" style="15" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="16.46484375" style="15" bestFit="1" customWidth="1"/>
     <col min="24" max="26" width="12.46484375" style="15" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="11.1328125" style="15" bestFit="1" customWidth="1"/>
-    <col min="28" max="33" width="9.06640625" style="15"/>
+    <col min="28" max="29" width="9.06640625" style="15"/>
+    <col min="30" max="30" width="16.796875" style="15" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="9.06640625" style="15"/>
     <col min="34" max="34" width="11.3984375" style="15" bestFit="1" customWidth="1"/>
     <col min="35" max="16384" width="9.06640625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A1" s="15" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.4">
@@ -1896,42 +2259,47 @@
       </c>
     </row>
     <row r="19" spans="1:33" ht="36.4" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.4">
+      <c r="O21" s="31" t="s">
+        <v>191</v>
+      </c>
+    </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.4">
-      <c r="A22" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="26"/>
-      <c r="Q22" s="26"/>
-      <c r="R22" s="26"/>
-      <c r="S22" s="26"/>
-      <c r="T22" s="26"/>
-      <c r="U22" s="26"/>
-      <c r="V22" s="26"/>
-      <c r="W22" s="26"/>
-      <c r="X22" s="26"/>
-      <c r="Y22" s="26"/>
-      <c r="Z22" s="26"/>
-      <c r="AA22" s="26"/>
-      <c r="AB22" s="26"/>
-      <c r="AC22" s="26"/>
-      <c r="AD22" s="26"/>
-      <c r="AE22" s="26"/>
-      <c r="AF22" s="26"/>
-      <c r="AG22" s="27"/>
+      <c r="A22" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="34"/>
+      <c r="P22" s="34"/>
+      <c r="Q22" s="34"/>
+      <c r="R22" s="34"/>
+      <c r="S22" s="34"/>
+      <c r="T22" s="34"/>
+      <c r="U22" s="34"/>
+      <c r="V22" s="34"/>
+      <c r="W22" s="34"/>
+      <c r="X22" s="34"/>
+      <c r="Y22" s="34"/>
+      <c r="Z22" s="34"/>
+      <c r="AA22" s="34"/>
+      <c r="AB22" s="34"/>
+      <c r="AC22" s="34"/>
+      <c r="AD22" s="34"/>
+      <c r="AE22" s="34"/>
+      <c r="AF22" s="34"/>
+      <c r="AG22" s="35"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A23" s="2"/>
@@ -2036,32 +2404,32 @@
       <c r="A24" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="5">
-        <v>1</v>
-      </c>
-      <c r="K24" s="5">
-        <v>1</v>
-      </c>
-      <c r="L24" s="5">
-        <v>1</v>
-      </c>
-      <c r="M24" s="5">
-        <v>1</v>
-      </c>
-      <c r="N24" s="5">
-        <v>1</v>
-      </c>
-      <c r="O24" s="5">
+      <c r="B24" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="29">
+        <v>1</v>
+      </c>
+      <c r="K24" s="29">
+        <v>1</v>
+      </c>
+      <c r="L24" s="29">
+        <v>1</v>
+      </c>
+      <c r="M24" s="29">
+        <v>1</v>
+      </c>
+      <c r="N24" s="27">
+        <v>1</v>
+      </c>
+      <c r="O24" s="27">
         <v>1</v>
       </c>
       <c r="P24" s="5">
@@ -2097,7 +2465,7 @@
       <c r="Z24" s="3">
         <v>10</v>
       </c>
-      <c r="AA24" s="3">
+      <c r="AA24" s="26">
         <v>11</v>
       </c>
       <c r="AB24" s="4">
@@ -2109,7 +2477,7 @@
       <c r="AD24" s="2">
         <v>14</v>
       </c>
-      <c r="AE24" s="14">
+      <c r="AE24" s="2">
         <v>15</v>
       </c>
       <c r="AF24" s="2">
@@ -2123,30 +2491,30 @@
       <c r="A25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="5">
-        <v>1</v>
-      </c>
-      <c r="K25" s="5">
-        <v>1</v>
-      </c>
-      <c r="L25" s="5">
-        <v>1</v>
-      </c>
-      <c r="M25" s="5">
-        <v>1</v>
-      </c>
-      <c r="N25" s="5">
-        <v>1</v>
-      </c>
-      <c r="O25" s="3">
+      <c r="B25" s="39"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="29">
+        <v>1</v>
+      </c>
+      <c r="K25" s="29">
+        <v>1</v>
+      </c>
+      <c r="L25" s="29">
+        <v>1</v>
+      </c>
+      <c r="M25" s="29">
+        <v>1</v>
+      </c>
+      <c r="N25" s="27">
+        <v>1</v>
+      </c>
+      <c r="O25" s="28">
         <v>1</v>
       </c>
       <c r="P25" s="3">
@@ -2182,7 +2550,7 @@
       <c r="Z25" s="3">
         <v>12</v>
       </c>
-      <c r="AA25" s="3">
+      <c r="AA25" s="26">
         <v>13</v>
       </c>
       <c r="AB25" s="4">
@@ -2194,7 +2562,7 @@
       <c r="AD25" s="2">
         <v>16</v>
       </c>
-      <c r="AE25" s="14">
+      <c r="AE25" s="2">
         <v>17</v>
       </c>
       <c r="AF25" s="2"/>
@@ -2204,30 +2572,30 @@
       <c r="A26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="5">
-        <v>1</v>
-      </c>
-      <c r="K26" s="5">
-        <v>1</v>
-      </c>
-      <c r="L26" s="5">
-        <v>1</v>
-      </c>
-      <c r="M26" s="3">
-        <v>1</v>
-      </c>
-      <c r="N26" s="3">
+      <c r="B26" s="39"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="29">
+        <v>1</v>
+      </c>
+      <c r="K26" s="29">
+        <v>1</v>
+      </c>
+      <c r="L26" s="29">
+        <v>1</v>
+      </c>
+      <c r="M26" s="30">
+        <v>1</v>
+      </c>
+      <c r="N26" s="28">
         <v>2</v>
       </c>
-      <c r="O26" s="3">
+      <c r="O26" s="28">
         <v>3</v>
       </c>
       <c r="P26" s="3">
@@ -2263,7 +2631,7 @@
       <c r="Z26" s="3">
         <v>14</v>
       </c>
-      <c r="AA26" s="3">
+      <c r="AA26" s="26">
         <v>15</v>
       </c>
       <c r="AB26" s="4">
@@ -2281,30 +2649,30 @@
       <c r="A27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="5">
-        <v>1</v>
-      </c>
-      <c r="K27" s="3">
-        <v>1</v>
-      </c>
-      <c r="L27" s="3">
+      <c r="B27" s="41"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="29">
+        <v>1</v>
+      </c>
+      <c r="K27" s="30">
+        <v>1</v>
+      </c>
+      <c r="L27" s="30">
         <v>2</v>
       </c>
-      <c r="M27" s="3">
+      <c r="M27" s="30">
         <v>3</v>
       </c>
-      <c r="N27" s="3">
+      <c r="N27" s="28">
         <v>4</v>
       </c>
-      <c r="O27" s="3">
+      <c r="O27" s="28">
         <v>5</v>
       </c>
       <c r="P27" s="3">
@@ -2340,7 +2708,7 @@
       <c r="Z27" s="3">
         <v>16</v>
       </c>
-      <c r="AA27" s="3">
+      <c r="AA27" s="26">
         <v>17</v>
       </c>
       <c r="AB27" s="2"/>
@@ -2386,41 +2754,41 @@
       <c r="AG28" s="19"/>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.4">
-      <c r="A29" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="26"/>
-      <c r="M29" s="26"/>
-      <c r="N29" s="26"/>
-      <c r="O29" s="26"/>
-      <c r="P29" s="26"/>
-      <c r="Q29" s="26"/>
-      <c r="R29" s="26"/>
-      <c r="S29" s="26"/>
-      <c r="T29" s="26"/>
-      <c r="U29" s="26"/>
-      <c r="V29" s="26"/>
-      <c r="W29" s="26"/>
-      <c r="X29" s="26"/>
-      <c r="Y29" s="26"/>
-      <c r="Z29" s="26"/>
-      <c r="AA29" s="26"/>
-      <c r="AB29" s="26"/>
-      <c r="AC29" s="26"/>
-      <c r="AD29" s="26"/>
-      <c r="AE29" s="26"/>
-      <c r="AF29" s="26"/>
-      <c r="AG29" s="27"/>
+      <c r="A29" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="34"/>
+      <c r="L29" s="34"/>
+      <c r="M29" s="34"/>
+      <c r="N29" s="34"/>
+      <c r="O29" s="34"/>
+      <c r="P29" s="34"/>
+      <c r="Q29" s="34"/>
+      <c r="R29" s="34"/>
+      <c r="S29" s="34"/>
+      <c r="T29" s="34"/>
+      <c r="U29" s="34"/>
+      <c r="V29" s="34"/>
+      <c r="W29" s="34"/>
+      <c r="X29" s="34"/>
+      <c r="Y29" s="34"/>
+      <c r="Z29" s="34"/>
+      <c r="AA29" s="34"/>
+      <c r="AB29" s="34"/>
+      <c r="AC29" s="34"/>
+      <c r="AD29" s="34"/>
+      <c r="AE29" s="34"/>
+      <c r="AF29" s="34"/>
+      <c r="AG29" s="35"/>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A30" s="2"/>
@@ -2568,9 +2936,11 @@
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B32" s="2"/>
+        <v>113</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="C32" s="12" t="s">
         <v>27</v>
       </c>
@@ -2592,22 +2962,22 @@
       <c r="I32" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J32" s="3" t="s">
+      <c r="J32" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="K32" s="3" t="s">
+      <c r="K32" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="L32" s="3" t="s">
+      <c r="L32" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="M32" s="3" t="s">
+      <c r="M32" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="N32" s="3" t="s">
+      <c r="N32" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="O32" s="3" t="s">
+      <c r="O32" s="28" t="s">
         <v>32</v>
       </c>
       <c r="P32" s="3" t="s">
@@ -2643,7 +3013,7 @@
       <c r="Z32" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AA32" s="3" t="s">
+      <c r="AA32" s="26" t="s">
         <v>11</v>
       </c>
       <c r="AB32" s="4" t="s">
@@ -2667,79 +3037,81 @@
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B33" s="2"/>
+        <v>114</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>187</v>
+      </c>
       <c r="C33" s="12" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K33" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="J33" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="K33" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="L33" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="L33" s="3" t="s">
+      <c r="M33" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="M33" s="3" t="s">
+      <c r="N33" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="N33" s="3" t="s">
+      <c r="O33" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="O33" s="3" t="s">
+      <c r="P33" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="P33" s="3" t="s">
+      <c r="Q33" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="Q33" s="3" t="s">
+      <c r="R33" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="R33" s="3" t="s">
+      <c r="S33" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="S33" s="3" t="s">
+      <c r="T33" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="T33" s="3" t="s">
+      <c r="U33" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="U33" s="3" t="s">
+      <c r="V33" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="V33" s="3" t="s">
+      <c r="W33" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="W33" s="3" t="s">
+      <c r="X33" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="X33" s="3" t="s">
+      <c r="Y33" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="Y33" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z33" s="3" t="s">
+      <c r="Z33" s="26" t="s">
         <v>19</v>
       </c>
       <c r="AA33" s="4" t="s">
@@ -2761,41 +3133,41 @@
       <c r="AG33" s="2"/>
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.4">
-      <c r="A36" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="26"/>
-      <c r="J36" s="26"/>
-      <c r="K36" s="26"/>
-      <c r="L36" s="26"/>
-      <c r="M36" s="26"/>
-      <c r="N36" s="26"/>
-      <c r="O36" s="26"/>
-      <c r="P36" s="26"/>
-      <c r="Q36" s="26"/>
-      <c r="R36" s="26"/>
-      <c r="S36" s="26"/>
-      <c r="T36" s="26"/>
-      <c r="U36" s="26"/>
-      <c r="V36" s="26"/>
-      <c r="W36" s="26"/>
-      <c r="X36" s="26"/>
-      <c r="Y36" s="26"/>
-      <c r="Z36" s="26"/>
-      <c r="AA36" s="26"/>
-      <c r="AB36" s="26"/>
-      <c r="AC36" s="26"/>
-      <c r="AD36" s="26"/>
-      <c r="AE36" s="26"/>
-      <c r="AF36" s="26"/>
-      <c r="AG36" s="27"/>
+      <c r="A36" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="34"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="34"/>
+      <c r="L36" s="34"/>
+      <c r="M36" s="34"/>
+      <c r="N36" s="34"/>
+      <c r="O36" s="34"/>
+      <c r="P36" s="34"/>
+      <c r="Q36" s="34"/>
+      <c r="R36" s="34"/>
+      <c r="S36" s="34"/>
+      <c r="T36" s="34"/>
+      <c r="U36" s="34"/>
+      <c r="V36" s="34"/>
+      <c r="W36" s="34"/>
+      <c r="X36" s="34"/>
+      <c r="Y36" s="34"/>
+      <c r="Z36" s="34"/>
+      <c r="AA36" s="34"/>
+      <c r="AB36" s="34"/>
+      <c r="AC36" s="34"/>
+      <c r="AD36" s="34"/>
+      <c r="AE36" s="34"/>
+      <c r="AF36" s="34"/>
+      <c r="AG36" s="35"/>
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A37" s="2"/>
@@ -2901,20 +3273,22 @@
       <c r="A38" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="11">
-        <v>1</v>
-      </c>
-      <c r="D38" s="5">
-        <v>1</v>
-      </c>
-      <c r="E38" s="5">
-        <v>1</v>
-      </c>
-      <c r="F38" s="5">
-        <v>1</v>
-      </c>
-      <c r="G38" s="5">
+      <c r="B38" s="11">
+        <v>1</v>
+      </c>
+      <c r="C38" s="29">
+        <v>1</v>
+      </c>
+      <c r="D38" s="29">
+        <v>1</v>
+      </c>
+      <c r="E38" s="29">
+        <v>1</v>
+      </c>
+      <c r="F38" s="27">
+        <v>1</v>
+      </c>
+      <c r="G38" s="27">
         <v>1</v>
       </c>
       <c r="H38" s="5">
@@ -2950,7 +3324,7 @@
       <c r="R38" s="3">
         <v>10</v>
       </c>
-      <c r="S38" s="3">
+      <c r="S38" s="26">
         <v>11</v>
       </c>
       <c r="T38" s="4">
@@ -2985,20 +3359,22 @@
       <c r="A39" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="11">
-        <v>1</v>
-      </c>
-      <c r="D39" s="5">
-        <v>1</v>
-      </c>
-      <c r="E39" s="5">
-        <v>1</v>
-      </c>
-      <c r="F39" s="5">
-        <v>1</v>
-      </c>
-      <c r="G39" s="3">
+      <c r="B39" s="11">
+        <v>1</v>
+      </c>
+      <c r="C39" s="29">
+        <v>1</v>
+      </c>
+      <c r="D39" s="29">
+        <v>1</v>
+      </c>
+      <c r="E39" s="29">
+        <v>1</v>
+      </c>
+      <c r="F39" s="27">
+        <v>1</v>
+      </c>
+      <c r="G39" s="28">
         <v>1</v>
       </c>
       <c r="H39" s="3">
@@ -3034,7 +3410,7 @@
       <c r="R39" s="3">
         <v>12</v>
       </c>
-      <c r="S39" s="3">
+      <c r="S39" s="26">
         <v>13</v>
       </c>
       <c r="T39" s="4">
@@ -3065,20 +3441,22 @@
       <c r="A40" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="11">
-        <v>1</v>
-      </c>
-      <c r="D40" s="5">
-        <v>1</v>
-      </c>
-      <c r="E40" s="3">
-        <v>1</v>
-      </c>
-      <c r="F40" s="3">
+      <c r="B40" s="11">
+        <v>1</v>
+      </c>
+      <c r="C40" s="29">
+        <v>1</v>
+      </c>
+      <c r="D40" s="29">
+        <v>1</v>
+      </c>
+      <c r="E40" s="30">
+        <v>1</v>
+      </c>
+      <c r="F40" s="28">
         <v>2</v>
       </c>
-      <c r="G40" s="3">
+      <c r="G40" s="28">
         <v>3</v>
       </c>
       <c r="H40" s="3">
@@ -3114,7 +3492,7 @@
       <c r="R40" s="3">
         <v>14</v>
       </c>
-      <c r="S40" s="3">
+      <c r="S40" s="26">
         <v>15</v>
       </c>
       <c r="T40" s="4">
@@ -3141,20 +3519,22 @@
       <c r="A41" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="11">
-        <v>1</v>
-      </c>
-      <c r="D41" s="3">
+      <c r="B41" s="11">
+        <v>1</v>
+      </c>
+      <c r="C41" s="29">
+        <v>1</v>
+      </c>
+      <c r="D41" s="30">
         <v>2</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="30">
         <v>3</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F41" s="28">
         <v>4</v>
       </c>
-      <c r="G41" s="3">
+      <c r="G41" s="28">
         <v>5</v>
       </c>
       <c r="H41" s="3">
@@ -3190,7 +3570,7 @@
       <c r="R41" s="3">
         <v>16</v>
       </c>
-      <c r="S41" s="3">
+      <c r="S41" s="26">
         <v>17</v>
       </c>
       <c r="T41" s="2"/>
@@ -3219,45 +3599,45 @@
       <c r="AH44"/>
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.4">
-      <c r="A45" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="26"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="26"/>
-      <c r="K45" s="26"/>
-      <c r="L45" s="26"/>
-      <c r="M45" s="26"/>
-      <c r="N45" s="26"/>
-      <c r="O45" s="26"/>
-      <c r="P45" s="26"/>
-      <c r="Q45" s="26"/>
-      <c r="R45" s="26"/>
-      <c r="S45" s="26"/>
-      <c r="T45" s="26"/>
-      <c r="U45" s="26"/>
-      <c r="V45" s="26"/>
-      <c r="W45" s="26"/>
-      <c r="X45" s="26"/>
-      <c r="Y45" s="26"/>
-      <c r="Z45" s="26"/>
-      <c r="AA45" s="26"/>
-      <c r="AB45" s="26"/>
-      <c r="AC45" s="26"/>
-      <c r="AD45" s="26"/>
-      <c r="AE45" s="26"/>
-      <c r="AF45" s="26"/>
-      <c r="AG45" s="27"/>
+      <c r="A45" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="B45" s="34"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="34"/>
+      <c r="G45" s="34"/>
+      <c r="H45" s="34"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
+      <c r="K45" s="34"/>
+      <c r="L45" s="34"/>
+      <c r="M45" s="34"/>
+      <c r="N45" s="34"/>
+      <c r="O45" s="34"/>
+      <c r="P45" s="34"/>
+      <c r="Q45" s="34"/>
+      <c r="R45" s="34"/>
+      <c r="S45" s="34"/>
+      <c r="T45" s="34"/>
+      <c r="U45" s="34"/>
+      <c r="V45" s="34"/>
+      <c r="W45" s="34"/>
+      <c r="X45" s="34"/>
+      <c r="Y45" s="34"/>
+      <c r="Z45" s="34"/>
+      <c r="AA45" s="34"/>
+      <c r="AB45" s="34"/>
+      <c r="AC45" s="34"/>
+      <c r="AD45" s="34"/>
+      <c r="AE45" s="34"/>
+      <c r="AF45" s="34"/>
+      <c r="AG45" s="35"/>
     </row>
     <row r="46" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
+      <c r="B46" s="9"/>
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
@@ -3275,7 +3655,7 @@
       <c r="Q46" s="9"/>
       <c r="R46" s="9"/>
       <c r="S46" s="9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
@@ -3294,22 +3674,24 @@
     </row>
     <row r="47" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B47" s="2"/>
-      <c r="C47" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D47" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C47" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="D47" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="E47" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="6" t="s">
+      <c r="F47" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="G47" s="6" t="s">
+      <c r="G47" s="28" t="s">
         <v>24</v>
       </c>
       <c r="H47" s="6" t="s">
@@ -3345,11 +3727,11 @@
       <c r="R47" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="S47" s="6" t="s">
+      <c r="S47" s="26" t="s">
         <v>36</v>
       </c>
       <c r="T47" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="U47" s="4" t="s">
         <v>38</v>
@@ -3378,62 +3760,64 @@
     </row>
     <row r="48" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B48" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="C48" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E48" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E48" s="6" t="s">
+      <c r="F48" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="F48" s="6" t="s">
+      <c r="G48" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G48" s="6" t="s">
+      <c r="H48" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="H48" s="6" t="s">
+      <c r="I48" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="I48" s="6" t="s">
+      <c r="J48" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="J48" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="K48" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="L48" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="L48" s="6" t="s">
+      <c r="M48" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="M48" s="6" t="s">
+      <c r="N48" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="N48" s="6" t="s">
+      <c r="O48" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="O48" s="6" t="s">
+      <c r="P48" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="P48" s="6" t="s">
+      <c r="Q48" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="Q48" s="6" t="s">
+      <c r="R48" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="R48" s="6" t="s">
+      <c r="S48" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="S48" s="4" t="s">
+      <c r="T48" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="T48" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="U48" s="2" t="s">
         <v>8</v>
@@ -3461,7 +3845,7 @@
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
@@ -3502,8 +3886,9 @@
       <c r="F50" s="19"/>
       <c r="G50" s="19"/>
       <c r="H50" s="19"/>
-      <c r="I50" s="19"/>
-      <c r="J50" s="19"/>
+      <c r="J50" s="28" t="s">
+        <v>186</v>
+      </c>
       <c r="K50" s="19"/>
       <c r="L50" s="19"/>
       <c r="M50" s="19"/>
@@ -3516,41 +3901,41 @@
       <c r="AH50"/>
     </row>
     <row r="51" spans="1:34" x14ac:dyDescent="0.4">
-      <c r="A51" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="B51" s="26"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="26"/>
-      <c r="H51" s="26"/>
-      <c r="I51" s="26"/>
-      <c r="J51" s="26"/>
-      <c r="K51" s="26"/>
-      <c r="L51" s="26"/>
-      <c r="M51" s="26"/>
-      <c r="N51" s="26"/>
-      <c r="O51" s="26"/>
-      <c r="P51" s="26"/>
-      <c r="Q51" s="26"/>
-      <c r="R51" s="26"/>
-      <c r="S51" s="26"/>
-      <c r="T51" s="26"/>
-      <c r="U51" s="26"/>
-      <c r="V51" s="26"/>
-      <c r="W51" s="26"/>
-      <c r="X51" s="26"/>
-      <c r="Y51" s="26"/>
-      <c r="Z51" s="26"/>
-      <c r="AA51" s="26"/>
-      <c r="AB51" s="26"/>
-      <c r="AC51" s="26"/>
-      <c r="AD51" s="26"/>
-      <c r="AE51" s="26"/>
-      <c r="AF51" s="26"/>
-      <c r="AG51" s="27"/>
+      <c r="A51" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="B51" s="34"/>
+      <c r="C51" s="34"/>
+      <c r="D51" s="34"/>
+      <c r="E51" s="34"/>
+      <c r="F51" s="34"/>
+      <c r="G51" s="34"/>
+      <c r="H51" s="34"/>
+      <c r="I51" s="34"/>
+      <c r="J51" s="34"/>
+      <c r="K51" s="34"/>
+      <c r="L51" s="34"/>
+      <c r="M51" s="34"/>
+      <c r="N51" s="34"/>
+      <c r="O51" s="34"/>
+      <c r="P51" s="34"/>
+      <c r="Q51" s="34"/>
+      <c r="R51" s="34"/>
+      <c r="S51" s="34"/>
+      <c r="T51" s="34"/>
+      <c r="U51" s="34"/>
+      <c r="V51" s="34"/>
+      <c r="W51" s="34"/>
+      <c r="X51" s="34"/>
+      <c r="Y51" s="34"/>
+      <c r="Z51" s="34"/>
+      <c r="AA51" s="34"/>
+      <c r="AB51" s="34"/>
+      <c r="AC51" s="34"/>
+      <c r="AD51" s="34"/>
+      <c r="AE51" s="34"/>
+      <c r="AF51" s="34"/>
+      <c r="AG51" s="35"/>
       <c r="AH51"/>
     </row>
     <row r="52" spans="1:34" x14ac:dyDescent="0.4">
@@ -3654,31 +4039,33 @@
     </row>
     <row r="53" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A53" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B53" s="2"/>
-      <c r="C53" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D53" s="10" t="s">
+      <c r="C53" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E53" s="10" t="s">
+      <c r="D53" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="F53" s="10" t="s">
+      <c r="E53" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G53" s="10" t="s">
+      <c r="F53" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="H53" s="10" t="s">
+      <c r="G53" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="I53" s="10" t="s">
+      <c r="H53" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="J53" s="10" t="s">
+      <c r="I53" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="J53" s="28" t="s">
         <v>27</v>
       </c>
       <c r="K53" s="10" t="s">
@@ -3711,13 +4098,13 @@
       <c r="T53" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="U53" s="10" t="s">
+      <c r="U53" s="26" t="s">
         <v>38</v>
       </c>
       <c r="V53" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="W53" s="10" t="s">
+      <c r="W53" s="26" t="s">
         <v>40</v>
       </c>
       <c r="X53" s="4" t="s">
@@ -3753,77 +4140,79 @@
     </row>
     <row r="54" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A54" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B54" s="2"/>
-      <c r="C54" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F54" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G54" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="H54" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="I54" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="J54" s="10" t="s">
-        <v>55</v>
+        <v>114</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="C54" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="D54" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="E54" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="F54" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="G54" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="H54" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="I54" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="J54" s="28" t="s">
+        <v>187</v>
       </c>
       <c r="K54" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="L54" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="L54" s="10" t="s">
+      <c r="M54" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="M54" s="10" t="s">
+      <c r="N54" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="N54" s="10" t="s">
+      <c r="O54" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="O54" s="10" t="s">
+      <c r="P54" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="P54" s="10" t="s">
+      <c r="Q54" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="Q54" s="10" t="s">
+      <c r="R54" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="R54" s="10" t="s">
+      <c r="S54" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="S54" s="10" t="s">
+      <c r="T54" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="T54" s="10" t="s">
+      <c r="U54" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="U54" s="10" t="s">
+      <c r="V54" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="V54" s="10" t="s">
+      <c r="W54" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="W54" s="10" t="s">
+      <c r="X54" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="X54" s="4" t="s">
+      <c r="Y54" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="Y54" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="Z54" s="7" t="s">
         <v>19</v>
@@ -3848,31 +4237,33 @@
     </row>
     <row r="55" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A55" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C55" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="D55" s="10" t="s">
+      <c r="D55" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E55" s="10" t="s">
+      <c r="E55" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="F55" s="10" t="s">
+      <c r="F55" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="G55" s="10" t="s">
+      <c r="G55" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="H55" s="10" t="s">
+      <c r="H55" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="I55" s="10" t="s">
+      <c r="I55" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="J55" s="10" t="s">
+      <c r="J55" s="28" t="s">
         <v>27</v>
       </c>
       <c r="K55" s="10" t="s">
@@ -3905,13 +4296,13 @@
       <c r="T55" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="U55" s="10" t="s">
+      <c r="U55" s="26" t="s">
         <v>38</v>
       </c>
       <c r="V55" s="10">
         <v>14</v>
       </c>
-      <c r="W55" s="10">
+      <c r="W55" s="26">
         <v>15</v>
       </c>
       <c r="X55" s="4">
@@ -3931,62 +4322,64 @@
     </row>
     <row r="56" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B56" s="2"/>
-      <c r="C56" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="C56" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="D56" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="D56" s="10" t="s">
+      <c r="E56" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E56" s="10" t="s">
+      <c r="F56" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="F56" s="10" t="s">
+      <c r="G56" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="G56" s="10" t="s">
+      <c r="H56" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="H56" s="10" t="s">
+      <c r="I56" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="I56" s="10" t="s">
+      <c r="J56" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="J56" s="10" t="s">
+      <c r="K56" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="K56" s="10" t="s">
+      <c r="L56" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="L56" s="10" t="s">
+      <c r="M56" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="M56" s="10" t="s">
+      <c r="N56" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="N56" s="10" t="s">
+      <c r="O56" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="O56" s="10" t="s">
+      <c r="P56" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="P56" s="10" t="s">
+      <c r="Q56" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="Q56" s="10" t="s">
+      <c r="R56" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="R56" s="10" t="s">
+      <c r="S56" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="S56" s="10" t="s">
+      <c r="T56" s="10" t="s">
         <v>64</v>
-      </c>
-      <c r="T56" s="10" t="s">
-        <v>65</v>
       </c>
       <c r="U56" s="10" t="s">
         <v>8</v>
@@ -3994,7 +4387,7 @@
       <c r="V56" s="10">
         <v>16</v>
       </c>
-      <c r="W56" s="10">
+      <c r="W56" s="26">
         <v>17</v>
       </c>
       <c r="X56" s="7"/>
@@ -4010,46 +4403,46 @@
       <c r="AH56"/>
     </row>
     <row r="59" spans="1:34" x14ac:dyDescent="0.4">
-      <c r="A59" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="B59" s="26"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="26"/>
-      <c r="E59" s="26"/>
-      <c r="F59" s="26"/>
-      <c r="G59" s="26"/>
-      <c r="H59" s="26"/>
-      <c r="I59" s="26"/>
-      <c r="J59" s="26"/>
-      <c r="K59" s="26"/>
-      <c r="L59" s="26"/>
-      <c r="M59" s="26"/>
-      <c r="N59" s="26"/>
-      <c r="O59" s="26"/>
-      <c r="P59" s="26"/>
-      <c r="Q59" s="26"/>
-      <c r="R59" s="26"/>
-      <c r="S59" s="26"/>
-      <c r="T59" s="26"/>
-      <c r="U59" s="26"/>
-      <c r="V59" s="26"/>
-      <c r="W59" s="26"/>
-      <c r="X59" s="26"/>
-      <c r="Y59" s="26"/>
-      <c r="Z59" s="26"/>
-      <c r="AA59" s="26"/>
-      <c r="AB59" s="26"/>
-      <c r="AC59" s="26"/>
-      <c r="AD59" s="26"/>
-      <c r="AE59" s="26"/>
-      <c r="AF59" s="26"/>
-      <c r="AG59" s="27"/>
+      <c r="A59" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="B59" s="34"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="34"/>
+      <c r="F59" s="34"/>
+      <c r="G59" s="34"/>
+      <c r="H59" s="34"/>
+      <c r="I59" s="34"/>
+      <c r="J59" s="34"/>
+      <c r="K59" s="34"/>
+      <c r="L59" s="34"/>
+      <c r="M59" s="34"/>
+      <c r="N59" s="34"/>
+      <c r="O59" s="34"/>
+      <c r="P59" s="34"/>
+      <c r="Q59" s="34"/>
+      <c r="R59" s="34"/>
+      <c r="S59" s="34"/>
+      <c r="T59" s="34"/>
+      <c r="U59" s="34"/>
+      <c r="V59" s="34"/>
+      <c r="W59" s="34"/>
+      <c r="X59" s="34"/>
+      <c r="Y59" s="34"/>
+      <c r="Z59" s="34"/>
+      <c r="AA59" s="34"/>
+      <c r="AB59" s="34"/>
+      <c r="AC59" s="34"/>
+      <c r="AD59" s="34"/>
+      <c r="AE59" s="34"/>
+      <c r="AF59" s="34"/>
+      <c r="AG59" s="35"/>
       <c r="AH59"/>
     </row>
     <row r="60" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
+      <c r="B60" s="9"/>
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
@@ -4070,10 +4463,10 @@
       <c r="T60" s="9"/>
       <c r="U60" s="9"/>
       <c r="V60" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="W60" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="X60" s="2"/>
       <c r="Y60" s="2"/>
@@ -4188,77 +4581,79 @@
     </row>
     <row r="62" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A62" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B62" s="2"/>
-      <c r="C62" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="C62" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="D62" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="E62" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="D62" s="10" t="s">
+      <c r="F62" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="E62" s="10" t="s">
+      <c r="G62" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="H62" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="F62" s="10" t="s">
+      <c r="I62" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="G62" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="H62" s="10" t="s">
+      <c r="J62" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="I62" s="10" t="s">
+      <c r="K62" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="J62" s="10" t="s">
+      <c r="L62" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="K62" s="10" t="s">
+      <c r="M62" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="L62" s="10" t="s">
+      <c r="N62" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="M62" s="10" t="s">
+      <c r="O62" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="N62" s="10" t="s">
+      <c r="P62" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="O62" s="10" t="s">
+      <c r="Q62" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="P62" s="10" t="s">
+      <c r="R62" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="Q62" s="10" t="s">
+      <c r="S62" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="R62" s="10" t="s">
+      <c r="T62" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="S62" s="10" t="s">
+      <c r="U62" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="T62" s="10" t="s">
+      <c r="V62" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="U62" s="10" t="s">
+      <c r="W62" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="V62" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="W62" s="10" t="s">
-        <v>114</v>
-      </c>
       <c r="X62" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="Y62" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Z62" s="7" t="s">
         <v>10</v>
@@ -4272,13 +4667,13 @@
       <c r="AC62" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="AD62" s="2">
+      <c r="AD62" s="7">
         <v>14</v>
       </c>
-      <c r="AE62" s="2">
+      <c r="AE62" s="7">
         <v>15</v>
       </c>
-      <c r="AF62" s="2">
+      <c r="AF62" s="7">
         <v>16</v>
       </c>
       <c r="AG62" s="2">
@@ -4287,74 +4682,76 @@
     </row>
     <row r="63" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B63" s="2"/>
-      <c r="C63" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B63" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="C63" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="D63" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="E63" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="D63" s="10" t="s">
+      <c r="F63" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="E63" s="10" t="s">
+      <c r="G63" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="F63" s="10" t="s">
+      <c r="H63" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G63" s="10" t="s">
+      <c r="I63" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="H63" s="10" t="s">
+      <c r="J63" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="I63" s="10" t="s">
+      <c r="K63" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="J63" s="10" t="s">
+      <c r="L63" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="K63" s="10" t="s">
+      <c r="M63" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="L63" s="10" t="s">
+      <c r="N63" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="M63" s="10" t="s">
+      <c r="O63" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="N63" s="10" t="s">
+      <c r="P63" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="O63" s="10" t="s">
+      <c r="Q63" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="P63" s="10" t="s">
+      <c r="R63" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="Q63" s="10" t="s">
+      <c r="S63" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="R63" s="10" t="s">
+      <c r="T63" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="S63" s="10" t="s">
+      <c r="U63" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="T63" s="10" t="s">
+      <c r="V63" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="U63" s="10" t="s">
+      <c r="W63" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="V63" s="10" t="s">
+      <c r="X63" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="W63" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="X63" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="Y63" s="7" t="s">
         <v>8</v>
@@ -4363,10 +4760,10 @@
         <v>19</v>
       </c>
       <c r="AA63" s="7" t="s">
-        <v>18</v>
+        <v>144</v>
       </c>
       <c r="AB63" s="7" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
       <c r="AC63" s="7" t="s">
         <v>8</v>
@@ -4377,20 +4774,379 @@
       <c r="AE63" s="7">
         <v>17</v>
       </c>
-      <c r="AF63" s="7" t="s">
+      <c r="AF63" s="7"/>
+      <c r="AG63" s="7"/>
+    </row>
+    <row r="64" spans="1:34" x14ac:dyDescent="0.4">
+      <c r="A64" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="B64" s="34"/>
+      <c r="C64" s="34"/>
+      <c r="D64" s="34"/>
+      <c r="E64" s="34"/>
+      <c r="F64" s="34"/>
+      <c r="G64" s="34"/>
+      <c r="H64" s="34"/>
+      <c r="I64" s="34"/>
+      <c r="J64" s="34"/>
+      <c r="K64" s="34"/>
+      <c r="L64" s="34"/>
+      <c r="M64" s="34"/>
+      <c r="N64" s="34"/>
+      <c r="O64" s="34"/>
+      <c r="P64" s="34"/>
+      <c r="Q64" s="34"/>
+      <c r="R64" s="34"/>
+      <c r="S64" s="34"/>
+      <c r="T64" s="34"/>
+      <c r="U64" s="34"/>
+      <c r="V64" s="34"/>
+      <c r="W64" s="34"/>
+      <c r="X64" s="34"/>
+      <c r="Y64" s="34"/>
+      <c r="Z64" s="34"/>
+      <c r="AA64" s="34"/>
+      <c r="AB64" s="34"/>
+      <c r="AC64" s="34"/>
+      <c r="AD64" s="34"/>
+      <c r="AE64" s="34"/>
+      <c r="AF64" s="34"/>
+      <c r="AG64" s="35"/>
+    </row>
+    <row r="65" spans="1:34" x14ac:dyDescent="0.4">
+      <c r="A65" s="2"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="9"/>
+      <c r="H65" s="9"/>
+      <c r="I65" s="9"/>
+      <c r="J65" s="9"/>
+      <c r="K65" s="9"/>
+      <c r="L65" s="9"/>
+      <c r="M65" s="9"/>
+      <c r="N65" s="9"/>
+      <c r="O65" s="9"/>
+      <c r="P65" s="9"/>
+      <c r="Q65" s="9"/>
+      <c r="R65" s="9"/>
+      <c r="S65" s="9"/>
+      <c r="T65" s="9"/>
+      <c r="U65" s="9"/>
+      <c r="V65" s="9"/>
+      <c r="W65" s="9"/>
+      <c r="X65" s="9"/>
+      <c r="Y65" s="9"/>
+      <c r="Z65" s="9"/>
+      <c r="AA65" s="9"/>
+      <c r="AB65" s="9"/>
+      <c r="AC65" s="9"/>
+      <c r="AD65" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE65" s="2"/>
+      <c r="AF65" s="2"/>
+      <c r="AG65" s="2"/>
+    </row>
+    <row r="66" spans="1:34" x14ac:dyDescent="0.4">
+      <c r="A66" s="2"/>
+      <c r="B66" s="1">
+        <v>31</v>
+      </c>
+      <c r="C66" s="1">
+        <v>30</v>
+      </c>
+      <c r="D66" s="1">
+        <v>29</v>
+      </c>
+      <c r="E66" s="1">
+        <v>28</v>
+      </c>
+      <c r="F66" s="1">
+        <v>27</v>
+      </c>
+      <c r="G66" s="1">
+        <v>26</v>
+      </c>
+      <c r="H66" s="1">
+        <v>25</v>
+      </c>
+      <c r="I66" s="1">
+        <v>24</v>
+      </c>
+      <c r="J66" s="1">
+        <v>23</v>
+      </c>
+      <c r="K66" s="1">
+        <v>22</v>
+      </c>
+      <c r="L66" s="1">
+        <v>21</v>
+      </c>
+      <c r="M66" s="1">
+        <v>20</v>
+      </c>
+      <c r="N66" s="1">
+        <v>19</v>
+      </c>
+      <c r="O66" s="1">
+        <v>18</v>
+      </c>
+      <c r="P66" s="1">
+        <v>17</v>
+      </c>
+      <c r="Q66" s="1">
+        <v>16</v>
+      </c>
+      <c r="R66" s="1">
+        <v>15</v>
+      </c>
+      <c r="S66" s="1">
+        <v>14</v>
+      </c>
+      <c r="T66" s="1">
+        <v>13</v>
+      </c>
+      <c r="U66" s="1">
+        <v>12</v>
+      </c>
+      <c r="V66" s="1">
+        <v>11</v>
+      </c>
+      <c r="W66" s="1">
+        <v>10</v>
+      </c>
+      <c r="X66" s="1">
+        <v>9</v>
+      </c>
+      <c r="Y66" s="1">
         <v>8</v>
       </c>
-      <c r="AG63" s="7" t="s">
+      <c r="Z66" s="1">
+        <v>7</v>
+      </c>
+      <c r="AA66" s="1">
+        <v>6</v>
+      </c>
+      <c r="AB66" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC66" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD66" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE66" s="1">
+        <v>2</v>
+      </c>
+      <c r="AF66" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG66" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:34" x14ac:dyDescent="0.4">
+      <c r="A67" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B67" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="I67" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="J67" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="K67" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="L67" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="M67" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="N67" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="O67" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="P67" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q67" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="R67" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="S67" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="T67" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="U67" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="V67" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="W67" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="X67" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y67" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z67" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA67" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB67" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC67" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD67" s="4">
+        <v>14</v>
+      </c>
+      <c r="AE67" s="14">
+        <v>15</v>
+      </c>
+      <c r="AF67" s="2">
+        <v>16</v>
+      </c>
+      <c r="AG67" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:34" x14ac:dyDescent="0.4">
+      <c r="A68" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B68" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="I68" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="J68" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="K68" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="L68" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="M68" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="N68" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="O68" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="P68" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q68" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="R68" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="S68" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="T68" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="U68" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="V68" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="W68" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="X68" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Y68" s="14" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.4">
-      <c r="A65" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="B65" s="15" t="s">
-        <v>148</v>
-      </c>
+      <c r="Z68" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA68" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB68" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC68" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD68" s="4">
+        <v>16</v>
+      </c>
+      <c r="AE68" s="14">
+        <v>17</v>
+      </c>
+      <c r="AF68" s="7"/>
+      <c r="AG68" s="7"/>
     </row>
     <row r="70" spans="1:34" x14ac:dyDescent="0.4">
       <c r="AH70"/>
@@ -4400,53 +5156,53 @@
     </row>
     <row r="73" spans="1:34" x14ac:dyDescent="0.4">
       <c r="B73" s="15" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="74" spans="1:34" x14ac:dyDescent="0.4">
-      <c r="A74" s="24" t="s">
+      <c r="A74" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="B74" s="18">
+        <v>1</v>
+      </c>
+      <c r="C74" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="B74" s="18">
-        <v>1</v>
-      </c>
-      <c r="C74" s="15" t="s">
-        <v>126</v>
-      </c>
     </row>
     <row r="75" spans="1:34" x14ac:dyDescent="0.4">
-      <c r="A75" s="24"/>
+      <c r="A75" s="32"/>
       <c r="B75" s="20"/>
       <c r="C75" s="15" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="76" spans="1:34" x14ac:dyDescent="0.4">
-      <c r="A76" s="24"/>
+      <c r="A76" s="32"/>
       <c r="B76" s="21"/>
       <c r="C76" s="15" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="77" spans="1:34" x14ac:dyDescent="0.4">
-      <c r="A77" s="24"/>
+      <c r="A77" s="32"/>
       <c r="B77" s="15" t="s">
         <v>8</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="78" spans="1:34" x14ac:dyDescent="0.4">
-      <c r="A78" s="24"/>
+      <c r="A78" s="32"/>
       <c r="B78" s="15" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="79" spans="1:34" x14ac:dyDescent="0.4">
@@ -4454,7 +5210,7 @@
         <v>27</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="80" spans="1:34" x14ac:dyDescent="0.4">
@@ -4462,18 +5218,34 @@
         <v>27</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B83" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="C83" s="24"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B81" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C81" s="15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B82" s="26">
+        <v>17</v>
+      </c>
+      <c r="C82" s="15" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B87" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="C87" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B83:C83"/>
+  <mergeCells count="10">
+    <mergeCell ref="B87:C87"/>
     <mergeCell ref="A22:AG22"/>
     <mergeCell ref="A29:AG29"/>
     <mergeCell ref="A36:AG36"/>
@@ -4481,6 +5253,8 @@
     <mergeCell ref="A51:AG51"/>
     <mergeCell ref="A59:AG59"/>
     <mergeCell ref="A74:A78"/>
+    <mergeCell ref="A64:AG64"/>
+    <mergeCell ref="B24:I27"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>